<commit_message>
CHARMS - Update to RAS screener verifications in Native View
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/RASScenario_Consent_Age_11-13.xlsx
+++ b/src/test/java/CHARMS/resources/RASScenario_Consent_Age_11-13.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzipovay2/AquaProjects/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AE0B07-B977-6147-B8D4-55C6563DE8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8E620F-3B1A-5D49-B84C-C0222D492C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" activeTab="1" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
   </bookViews>
@@ -1636,8 +1636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAA49E6-03DB-BC47-B34D-065780B05137}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>